<commit_message>
updated min size of submit widget from 100 to 150
</commit_message>
<xml_diff>
--- a/rat.xlsx
+++ b/rat.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Esports\Collegiate\Drexel\2022-2023\DGA\PUGs-Power-Rankings\pugs-ranking\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54DE2D8-0975-408B-BE14-AC68CE5D8905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="20777" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>T1</t>
   </si>
@@ -70,80 +64,101 @@
     <t>High</t>
   </si>
   <si>
+    <t>LEOOW</t>
+  </si>
+  <si>
+    <t>RH77</t>
+  </si>
+  <si>
+    <t>BIGGIECHEESE</t>
+  </si>
+  <si>
+    <t>SEPPUNII</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
+  </si>
+  <si>
     <t>OPTIMALSHOT</t>
   </si>
   <si>
+    <t>TROOG</t>
+  </si>
+  <si>
+    <t>YAMISGEY</t>
+  </si>
+  <si>
+    <t>ALCHEMIST</t>
+  </si>
+  <si>
+    <t>&lt;-- DATA NOT YET RAN</t>
+  </si>
+  <si>
+    <t>NUMNUMS22</t>
+  </si>
+  <si>
+    <t>BEARABLEDOG</t>
+  </si>
+  <si>
+    <t>JEFFGOLDBLUM</t>
+  </si>
+  <si>
+    <t>DRAGONDAGGER</t>
+  </si>
+  <si>
+    <t>PEANUT</t>
+  </si>
+  <si>
+    <t>CEEBEE</t>
+  </si>
+  <si>
+    <t>ITSGAMBL3R</t>
+  </si>
+  <si>
+    <t>PESTCONTROL</t>
+  </si>
+  <si>
+    <t>FURARC</t>
+  </si>
+  <si>
+    <t>SPONTY</t>
+  </si>
+  <si>
+    <t>UNWRITTEN</t>
+  </si>
+  <si>
     <t>WULGARR</t>
   </si>
   <si>
+    <t>UNFEATURED</t>
+  </si>
+  <si>
+    <t>THEPKFACTOR</t>
+  </si>
+  <si>
+    <t>ETERNALSPARK</t>
+  </si>
+  <si>
+    <t>BENANATOR876</t>
+  </si>
+  <si>
+    <t>CDOG</t>
+  </si>
+  <si>
+    <t>IOWNSWAG</t>
+  </si>
+  <si>
+    <t>STAZER</t>
+  </si>
+  <si>
     <t>RATGUN</t>
-  </si>
-  <si>
-    <t>UNFEATURED</t>
-  </si>
-  <si>
-    <t>PESTCONTROL</t>
-  </si>
-  <si>
-    <t>JEFFGOLDBLUM</t>
-  </si>
-  <si>
-    <t>PEANUT</t>
-  </si>
-  <si>
-    <t>ETERNALSPARK</t>
-  </si>
-  <si>
-    <t>SPONTY</t>
-  </si>
-  <si>
-    <t>BENANATOR876</t>
-  </si>
-  <si>
-    <t>&lt;-- DATA NOT YET RAN</t>
-  </si>
-  <si>
-    <t>NUMNUMS22</t>
-  </si>
-  <si>
-    <t>BEARABLEDOG</t>
-  </si>
-  <si>
-    <t>DRAGONDAGGER</t>
-  </si>
-  <si>
-    <t>CEEBEE</t>
-  </si>
-  <si>
-    <t>ITSGAMBL3R</t>
-  </si>
-  <si>
-    <t>FURARC</t>
-  </si>
-  <si>
-    <t>UNWRITTEN</t>
-  </si>
-  <si>
-    <t>THEPKFACTOR</t>
-  </si>
-  <si>
-    <t>CDOG</t>
-  </si>
-  <si>
-    <t>IOWNSWAG</t>
-  </si>
-  <si>
-    <t>STAZER</t>
-  </si>
-  <si>
-    <t>2636</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,14 +221,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -260,7 +267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,27 +299,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,24 +333,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,16 +508,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,14 +565,44 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
       <c r="L2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="L3" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="L3" t="s">
-        <v>27</v>
       </c>
       <c r="M3">
         <v>4000</v>
@@ -618,9 +617,9 @@
         <v>4450</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16">
       <c r="L4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4">
         <v>4400</v>
@@ -635,9 +634,9 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16">
       <c r="L5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="M5">
         <v>4314</v>
@@ -652,7 +651,7 @@
         <v>4314</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16">
       <c r="L6" t="s">
         <v>29</v>
       </c>
@@ -669,9 +668,9 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16">
       <c r="L7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M7">
         <v>3850</v>
@@ -686,9 +685,9 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16">
       <c r="L8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M8">
         <v>3900</v>
@@ -703,9 +702,9 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16">
       <c r="L9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M9">
         <v>3800</v>
@@ -720,9 +719,9 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16">
       <c r="L10" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="M10">
         <v>4000</v>
@@ -737,9 +736,9 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16">
       <c r="L11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M11">
         <v>3850</v>
@@ -754,9 +753,9 @@
         <v>4150</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16">
       <c r="L12" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="M12">
         <v>4100</v>
@@ -771,9 +770,9 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16">
       <c r="L13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M13">
         <v>3200</v>
@@ -788,9 +787,9 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16">
       <c r="L14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="M14">
         <v>3536</v>
@@ -805,9 +804,9 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16">
       <c r="L15" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="M15">
         <v>3850</v>
@@ -822,9 +821,9 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16">
       <c r="L16" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="M16">
         <v>3800</v>
@@ -839,9 +838,9 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="17" spans="12:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="12:16">
       <c r="L17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="M17">
         <v>3700</v>
@@ -856,9 +855,9 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="18" spans="12:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="12:16">
       <c r="L18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="M18">
         <v>3400</v>
@@ -873,9 +872,9 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="19" spans="12:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="12:16">
       <c r="L19" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="M19">
         <v>3050</v>
@@ -890,9 +889,9 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="20" spans="12:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="12:16">
       <c r="L20" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="M20">
         <v>2900</v>
@@ -907,9 +906,9 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="21" spans="12:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="12:16">
       <c r="L21" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="M21">
         <v>2400</v>
@@ -924,9 +923,9 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="22" spans="12:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="12:16">
       <c r="L22" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -941,9 +940,9 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="23" spans="12:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="12:16">
       <c r="L23" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="M23">
         <v>2400</v>
@@ -954,12 +953,11 @@
       <c r="O23">
         <v>2500</v>
       </c>
-      <c r="P23" t="s">
-        <v>38</v>
+      <c r="P23">
+        <v>2636</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>